<commit_message>
Added device cards and removed react
</commit_message>
<xml_diff>
--- a/application/seeds/template.xlsx
+++ b/application/seeds/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abog.CAANT\Documents\Projects\IOT\iotdash\application\seeds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{590FCC0B-0823-4D51-A4A4-1D645ADBF62A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32FDA6FD-ED58-49C1-8B60-1A14B5108F5C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9330" activeTab="1" xr2:uid="{596807CE-799C-4C6D-AC8D-77293DE32F5B}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>id</t>
   </si>
@@ -56,16 +56,69 @@
   </si>
   <si>
     <t>device_measurements</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>ab@g.com</t>
+  </si>
+  <si>
+    <t>cb@g.com</t>
+  </si>
+  <si>
+    <t>device_name</t>
+  </si>
+  <si>
+    <t>ESP1</t>
+  </si>
+  <si>
+    <t>ESP3</t>
+  </si>
+  <si>
+    <t>Ardunio</t>
+  </si>
+  <si>
+    <t>Telus</t>
+  </si>
+  <si>
+    <t>Rogers</t>
+  </si>
+  <si>
+    <t>Alpha</t>
+  </si>
+  <si>
+    <t>Beta</t>
+  </si>
+  <si>
+    <t>Gamma</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -88,13 +141,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -407,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9960C59-A745-4616-875B-29D4A9738CEF}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,22 +497,58 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{EA47296B-E2B3-41E8-BBC3-B0652CD5D402}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{7600F9B4-751B-40C9-B0D7-FBD6E7421D72}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4809DC4-D476-40D5-885F-1029BE395FB8}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -464,7 +556,98 @@
         <v>6</v>
       </c>
       <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated login page,fixed device card logic, have do do python dash now
</commit_message>
<xml_diff>
--- a/application/seeds/template.xlsx
+++ b/application/seeds/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abog.CAANT\Documents\Projects\IOT\iotdash\application\seeds\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\AB\Documents\Projects\IOT\iotdash\application\seeds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32FDA6FD-ED58-49C1-8B60-1A14B5108F5C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D90E9B-53EB-4BED-A437-B2F1E9CB1AF4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9330" activeTab="1" xr2:uid="{596807CE-799C-4C6D-AC8D-77293DE32F5B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{596807CE-799C-4C6D-AC8D-77293DE32F5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" r:id="rId1"/>
@@ -538,7 +538,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4809DC4-D476-40D5-885F-1029BE395FB8}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -659,7 +659,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8FE370D-4890-4BCD-B325-55DE47758301}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>